<commit_message>
fix: calander as calender
</commit_message>
<xml_diff>
--- a/apps/web/LanguagePack.xlsx
+++ b/apps/web/LanguagePack.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="115">
   <si>
     <t>namespace</t>
   </si>
@@ -57,10 +57,10 @@
     <t>홈</t>
   </si>
   <si>
-    <t>calander</t>
-  </si>
-  <si>
-    <t>Calander</t>
+    <t>calender</t>
+  </si>
+  <si>
+    <t>Calender</t>
   </si>
   <si>
     <t>달력</t>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>삭제</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>error</t>
@@ -1001,7 +1004,11 @@
       </c>
     </row>
     <row r="19" ht="16.5" customHeight="1"/>
-    <row r="20" ht="16.5" customHeight="1"/>
+    <row r="20" ht="16.5" customHeight="1">
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="21" ht="16.5" customHeight="1"/>
     <row r="22" ht="16.5" customHeight="1"/>
     <row r="23" ht="16.5" customHeight="1"/>
@@ -1010,190 +1017,190 @@
     <row r="26" ht="16.5" customHeight="1"/>
     <row r="27" ht="16.5" customHeight="1">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D27" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" ht="16.5" customHeight="1"/>
     <row r="29" ht="16.5" customHeight="1">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D29" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" ht="16.5" customHeight="1"/>
     <row r="31" ht="16.5" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D31" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" ht="16.5" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D32" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" ht="16.5" customHeight="1"/>
     <row r="34" ht="16.5" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D34" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" ht="16.5" customHeight="1"/>
     <row r="36" ht="16.5" customHeight="1">
       <c r="A36" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C36" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D36" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" ht="16.5" customHeight="1"/>
     <row r="38" ht="16.5" customHeight="1">
       <c r="A38" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B38" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C38" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D38" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" ht="16.5" customHeight="1">
       <c r="A39" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B39" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C39" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D39" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" ht="16.5" customHeight="1"/>
     <row r="41" ht="16.5" customHeight="1">
       <c r="A41" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B41" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C41" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D41" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" ht="16.5" customHeight="1">
       <c r="A42" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B42" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C42" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D42" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="43" ht="16.5" customHeight="1">
       <c r="A43" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B43" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C43" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D43" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" ht="16.5" customHeight="1">
       <c r="A44" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B44" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C44" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D44" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" ht="16.5" customHeight="1">
       <c r="A45" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B45" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C45" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D45" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46" ht="16.5" customHeight="1"/>
@@ -1202,13 +1209,13 @@
         <v>14</v>
       </c>
       <c r="B47" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C47" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D47" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" ht="16.5" customHeight="1">
@@ -1216,7 +1223,7 @@
         <v>14</v>
       </c>
       <c r="B48" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C48" t="s">
         <v>39</v>
@@ -1230,13 +1237,13 @@
         <v>14</v>
       </c>
       <c r="B49" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C49" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D49" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" ht="16.5" customHeight="1">
@@ -1244,99 +1251,99 @@
         <v>14</v>
       </c>
       <c r="B50" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C50" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D50" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="51" ht="16.5" customHeight="1"/>
     <row r="52" ht="16.5" customHeight="1"/>
     <row r="53" ht="16.5" customHeight="1">
       <c r="A53" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B53" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C53" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D53" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="54" ht="16.5" customHeight="1">
       <c r="A54" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B54" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C54" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D54" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55" ht="16.5" customHeight="1">
       <c r="A55" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B55" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C55" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D55" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" ht="16.5" customHeight="1">
       <c r="A56" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B56" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C56" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D56" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="57" ht="16.5" customHeight="1">
       <c r="A57" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B57" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C57" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D57" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="58" ht="16.5" customHeight="1">
       <c r="A58" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B58" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C58" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D58" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>